<commit_message>
2022.01.07 | Hu Wenqiang | Updated Comments
</commit_message>
<xml_diff>
--- a/高发人员户籍统计.xlsx
+++ b/高发人员户籍统计.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>省份</t>
   </si>
@@ -22,88 +22,106 @@
     <t>人数</t>
   </si>
   <si>
+    <t>四川省</t>
+  </si>
+  <si>
+    <t>河南省</t>
+  </si>
+  <si>
     <t>河北省</t>
   </si>
   <si>
+    <t>云南省</t>
+  </si>
+  <si>
+    <t>山东省</t>
+  </si>
+  <si>
+    <t>湖南省</t>
+  </si>
+  <si>
+    <t>广东省</t>
+  </si>
+  <si>
+    <t>黑龙江</t>
+  </si>
+  <si>
+    <t>山西省</t>
+  </si>
+  <si>
+    <t>辽宁省</t>
+  </si>
+  <si>
+    <t>内蒙古</t>
+  </si>
+  <si>
+    <t>湖北省</t>
+  </si>
+  <si>
     <t>陕西省</t>
   </si>
   <si>
-    <t>广东省</t>
-  </si>
-  <si>
-    <t>黑龙江</t>
+    <t>广西</t>
+  </si>
+  <si>
+    <t>安徽省</t>
+  </si>
+  <si>
+    <t>新疆</t>
+  </si>
+  <si>
+    <t>贵州省</t>
+  </si>
+  <si>
+    <t>江苏省</t>
   </si>
   <si>
     <t>江西省</t>
   </si>
   <si>
-    <t>山西省</t>
-  </si>
-  <si>
-    <t>江苏省</t>
+    <t>浙江省</t>
   </si>
   <si>
     <t>甘肃省</t>
   </si>
   <si>
-    <t>山东省</t>
-  </si>
-  <si>
-    <t>河南省</t>
-  </si>
-  <si>
-    <t>云南省</t>
-  </si>
-  <si>
-    <t>湖南省</t>
-  </si>
-  <si>
-    <t>辽宁省</t>
-  </si>
-  <si>
-    <t>湖北省</t>
+    <t>福建省</t>
+  </si>
+  <si>
+    <t>西藏自</t>
+  </si>
+  <si>
+    <t>吉林省</t>
   </si>
   <si>
     <t>青海省</t>
   </si>
   <si>
-    <t>新疆</t>
-  </si>
-  <si>
-    <t>内蒙古</t>
-  </si>
-  <si>
-    <t>贵州省</t>
-  </si>
-  <si>
-    <t>广西</t>
-  </si>
-  <si>
-    <t>四川省</t>
-  </si>
-  <si>
-    <t>安徽省</t>
+    <t>重庆市</t>
+  </si>
+  <si>
+    <t>海南省</t>
+  </si>
+  <si>
+    <t>宁夏</t>
+  </si>
+  <si>
+    <t>北京市</t>
   </si>
   <si>
     <t>上海市</t>
   </si>
   <si>
-    <t>福建省</t>
-  </si>
-  <si>
     <t>天津市</t>
   </si>
   <si>
-    <t>浙江省</t>
-  </si>
-  <si>
-    <t>吉林省</t>
-  </si>
-  <si>
-    <t>海南省</t>
-  </si>
-  <si>
-    <t>宁夏</t>
+    <t>香港</t>
+  </si>
+  <si>
+    <t>台湾省</t>
+  </si>
+  <si>
+    <t>澳门</t>
   </si>
   <si>
     <t>-1.0</t>
@@ -217,82 +235,82 @@
               <c:strCache>
                 <c:ptCount val="70"/>
                 <c:pt idx="0">
+                  <c:v>四川省</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>河南省</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>河北省</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>云南省</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>山东省</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>湖南省</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>广东省</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>黑龙江</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>山西省</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>辽宁省</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>内蒙古</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>湖北省</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>陕西省</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>广东省</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>黑龙江</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>江西省</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>山西省</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>江苏省</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>甘肃省</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>山东省</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>河南省</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>云南省</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>湖南省</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>辽宁省</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>湖北省</c:v>
+                  <c:v>广西</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>青海省</c:v>
+                  <c:v>安徽省</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>新疆</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>内蒙古</c:v>
+                  <c:v>贵州省</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>贵州省</c:v>
+                  <c:v>江苏省</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>广西</c:v>
+                  <c:v>江西省</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>四川省</c:v>
+                  <c:v>浙江省</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>安徽省</c:v>
+                  <c:v>甘肃省</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>上海市</c:v>
+                  <c:v>福建省</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>福建省</c:v>
+                  <c:v>西藏自</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>天津市</c:v>
+                  <c:v>吉林省</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>浙江省</c:v>
+                  <c:v>青海省</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>吉林省</c:v>
+                  <c:v>重庆市</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>海南省</c:v>
@@ -301,6 +319,24 @@
                   <c:v>宁夏</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>北京市</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>上海市</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>天津市</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>香港</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>台湾省</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>澳门</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>-1.0</c:v>
                 </c:pt>
               </c:strCache>
@@ -313,90 +349,108 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>186</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="32">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="33">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="34">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -803,7 +857,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -825,7 +879,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -833,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -841,7 +895,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -849,7 +903,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -857,7 +911,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -865,7 +919,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -873,7 +927,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -881,7 +935,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -889,7 +943,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -897,7 +951,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -905,7 +959,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -913,7 +967,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -921,7 +975,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -929,7 +983,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -937,7 +991,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -945,7 +999,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -953,7 +1007,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -961,7 +1015,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -969,7 +1023,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -977,7 +1031,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -985,7 +1039,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -993,7 +1047,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1001,7 +1055,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1009,7 +1063,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1017,7 +1071,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1025,7 +1079,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1033,7 +1087,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1041,7 +1095,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1049,6 +1103,54 @@
         <v>30</v>
       </c>
       <c r="B30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
         <v>0</v>
       </c>
     </row>

</xml_diff>